<commit_message>
Update all excel_loader.py files with correct column mappings
- CRM Dashboard: Updated to use correct column names and mapping
- ARC Dashboard: Updated to use correct column names and mapping
- Integration Dashboard: Updated to use correct column names and mapping
- Regression Testing Dashboard: Updated to use correct column names and mapping
- All loaders now properly handle 'Days to Go Live' calculation
- Updated Excel data source files with correct column names
- Added 'ALL' region support for all dashboards
- Improved error handling and logging
</commit_message>
<xml_diff>
--- a/Data Source/ARC Configurations.xlsx
+++ b/Data Source/ARC Configurations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tekion-my.sharepoint.com/personal/kthakur_tekion_com/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gautam/Desktop/Operations Hub/Data Source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5998100-67C3-4C63-AC23-40F6830D6759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB06F8C3-BFD8-7D41-9A65-C8AA4C3D6045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15140" yWindow="760" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="August Go Live" sheetId="13" r:id="rId1"/>
@@ -19,10 +19,10 @@
     <sheet name="NOV Go Live" sheetId="20" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'SEPT Go -Live'!$A$1:$N$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'August Go Live'!$A$1:$N$50</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'NOV Go Live'!$A$1:$T$50</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'OCT Go Live'!$A$1:$O$55</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'August Go Live'!$A$1:$N$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'SEPT Go -Live'!$A$1:$N$69</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -53,25 +53,25 @@
     <t>Go Live Date</t>
   </si>
   <si>
-    <t xml:space="preserve">Type of Implementation </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SIM </t>
-  </si>
-  <si>
-    <t>Dealership</t>
+    <t>Implementation Type</t>
+  </si>
+  <si>
+    <t>SIM Start Date</t>
+  </si>
+  <si>
+    <t>Dealership Name</t>
   </si>
   <si>
     <t>Region</t>
   </si>
   <si>
-    <t>Parts</t>
-  </si>
-  <si>
-    <t>Service</t>
-  </si>
-  <si>
-    <t>Accounting</t>
+    <t>Parts - Status</t>
+  </si>
+  <si>
+    <t>Service - Status</t>
+  </si>
+  <si>
+    <t>Accounting - Status</t>
   </si>
   <si>
     <t>CP LINK Created</t>
@@ -1274,7 +1274,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <charset val="1"/>
     </font>
     <font>
       <u/>
@@ -2111,28 +2110,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95E79EA-2A5E-49B1-8C96-B203C597B3C7}">
   <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="47" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="47" style="6" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" style="6" customWidth="1"/>
-    <col min="8" max="8" width="21.140625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="37.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="28.5703125" style="6" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" style="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="83.85546875" style="6" customWidth="1"/>
-    <col min="13" max="13" width="24.140625" style="6" customWidth="1"/>
-    <col min="14" max="15" width="28.28515625" style="19" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="19"/>
+    <col min="7" max="7" width="20.1640625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="21.1640625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="37.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="28.5" style="6" customWidth="1"/>
+    <col min="11" max="11" width="22.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="83.83203125" style="6" customWidth="1"/>
+    <col min="13" max="13" width="24.1640625" style="6" customWidth="1"/>
+    <col min="14" max="15" width="28.33203125" style="19" customWidth="1"/>
+    <col min="16" max="16384" width="9.1640625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" s="27" customFormat="1">
@@ -2224,7 +2223,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" ht="16">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -2430,7 +2429,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" ht="16">
       <c r="A8" s="3" t="s">
         <v>25</v>
       </c>
@@ -4101,54 +4100,54 @@
   <dimension ref="A1:Y69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C53" sqref="C53"/>
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="18.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="30.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="18.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="30.5" style="13" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="37" style="13" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="28" style="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="13"/>
+    <col min="14" max="14" width="22.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.1640625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="14" customFormat="1" ht="18.75">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:14" s="14" customFormat="1" ht="19">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="31" t="s">
@@ -4167,7 +4166,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="16" customFormat="1" ht="15.75">
+    <row r="2" spans="1:14" s="16" customFormat="1" ht="16">
       <c r="A2" s="16" t="s">
         <v>25</v>
       </c>
@@ -4205,7 +4204,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="16" customFormat="1" ht="15.75">
+    <row r="3" spans="1:14" s="16" customFormat="1" ht="16">
       <c r="A3" s="16" t="s">
         <v>25</v>
       </c>
@@ -4237,7 +4236,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="16" customFormat="1" ht="15.75">
+    <row r="4" spans="1:14" s="16" customFormat="1" ht="16">
       <c r="A4" s="16" t="s">
         <v>14</v>
       </c>
@@ -4272,7 +4271,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="16" customFormat="1" ht="15.75">
+    <row r="5" spans="1:14" s="16" customFormat="1" ht="16">
       <c r="A5" s="16" t="s">
         <v>14</v>
       </c>
@@ -4310,7 +4309,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="16" customFormat="1" ht="15.75">
+    <row r="6" spans="1:14" s="16" customFormat="1" ht="16">
       <c r="A6" s="16" t="s">
         <v>25</v>
       </c>
@@ -4345,7 +4344,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="16" customFormat="1" ht="15.75">
+    <row r="7" spans="1:14" s="16" customFormat="1" ht="16">
       <c r="A7" s="16" t="s">
         <v>14</v>
       </c>
@@ -4380,7 +4379,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="16" customFormat="1" ht="15.75">
+    <row r="8" spans="1:14" s="16" customFormat="1" ht="16">
       <c r="A8" s="16" t="s">
         <v>28</v>
       </c>
@@ -4415,7 +4414,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="16" customFormat="1" ht="15.75">
+    <row r="9" spans="1:14" s="16" customFormat="1" ht="16">
       <c r="A9" s="16" t="s">
         <v>28</v>
       </c>
@@ -4454,7 +4453,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="16" customFormat="1" ht="15.75">
+    <row r="10" spans="1:14" s="16" customFormat="1" ht="16">
       <c r="A10" s="16" t="s">
         <v>28</v>
       </c>
@@ -4493,7 +4492,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="16" customFormat="1" ht="15.75">
+    <row r="11" spans="1:14" s="16" customFormat="1" ht="16">
       <c r="A11" s="16" t="s">
         <v>41</v>
       </c>
@@ -4526,7 +4525,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="16" customFormat="1" ht="15.75">
+    <row r="12" spans="1:14" s="16" customFormat="1" ht="16">
       <c r="A12" s="16" t="s">
         <v>28</v>
       </c>
@@ -4561,7 +4560,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="16" customFormat="1" ht="15.75">
+    <row r="13" spans="1:14" s="16" customFormat="1" ht="16">
       <c r="A13" s="16" t="s">
         <v>14</v>
       </c>
@@ -4596,7 +4595,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="16" customFormat="1" ht="15.75">
+    <row r="14" spans="1:14" s="16" customFormat="1" ht="16">
       <c r="A14" s="16" t="s">
         <v>28</v>
       </c>
@@ -4631,7 +4630,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="16" customFormat="1" ht="15.75">
+    <row r="15" spans="1:14" s="16" customFormat="1" ht="16">
       <c r="A15" s="16" t="s">
         <v>14</v>
       </c>
@@ -4666,7 +4665,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="16" customFormat="1" ht="15.75">
+    <row r="16" spans="1:14" s="16" customFormat="1" ht="16">
       <c r="A16" s="16" t="s">
         <v>28</v>
       </c>
@@ -4704,7 +4703,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="17" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A17" s="16" t="s">
         <v>14</v>
       </c>
@@ -4739,7 +4738,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="18" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A18" s="16" t="s">
         <v>28</v>
       </c>
@@ -4777,7 +4776,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="19" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A19" s="16" t="s">
         <v>25</v>
       </c>
@@ -4812,7 +4811,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="20" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A20" s="16" t="s">
         <v>25</v>
       </c>
@@ -4847,7 +4846,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="21" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A21" s="16" t="s">
         <v>28</v>
       </c>
@@ -4885,7 +4884,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="22" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A22" s="16" t="s">
         <v>28</v>
       </c>
@@ -4920,7 +4919,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="23" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A23" s="16" t="s">
         <v>14</v>
       </c>
@@ -4955,7 +4954,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="24" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A24" s="16" t="s">
         <v>14</v>
       </c>
@@ -4990,7 +4989,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="25" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A25" s="16" t="s">
         <v>28</v>
       </c>
@@ -5025,7 +5024,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="26" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A26" s="16" t="s">
         <v>25</v>
       </c>
@@ -5063,7 +5062,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="27" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A27" s="16" t="s">
         <v>28</v>
       </c>
@@ -5101,7 +5100,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="28" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A28" s="16" t="s">
         <v>28</v>
       </c>
@@ -5139,7 +5138,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="29" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A29" s="16" t="s">
         <v>14</v>
       </c>
@@ -5177,7 +5176,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="30" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A30" s="16" t="s">
         <v>28</v>
       </c>
@@ -5215,7 +5214,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="31" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A31" s="16" t="s">
         <v>41</v>
       </c>
@@ -5247,7 +5246,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="32" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A32" s="16" t="s">
         <v>14</v>
       </c>
@@ -5279,7 +5278,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="33" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A33" s="16" t="s">
         <v>14</v>
       </c>
@@ -5314,7 +5313,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="34" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A34" s="16" t="s">
         <v>14</v>
       </c>
@@ -5349,7 +5348,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="35" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A35" s="16" t="s">
         <v>28</v>
       </c>
@@ -5384,7 +5383,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="36" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A36" s="16" t="s">
         <v>14</v>
       </c>
@@ -5419,7 +5418,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="37" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A37" s="16" t="s">
         <v>25</v>
       </c>
@@ -5454,7 +5453,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="38" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A38" s="16" t="s">
         <v>14</v>
       </c>
@@ -5489,7 +5488,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="39" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A39" s="16" t="s">
         <v>28</v>
       </c>
@@ -5524,7 +5523,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="40" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A40" s="16" t="s">
         <v>28</v>
       </c>
@@ -5559,7 +5558,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="41" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A41" s="16" t="s">
         <v>41</v>
       </c>
@@ -5591,7 +5590,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="42" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A42" s="16" t="s">
         <v>41</v>
       </c>
@@ -5623,7 +5622,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="43" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A43" s="16" t="s">
         <v>14</v>
       </c>
@@ -5661,7 +5660,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="44" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A44" s="16" t="s">
         <v>28</v>
       </c>
@@ -5699,7 +5698,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="45" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A45" s="16" t="s">
         <v>25</v>
       </c>
@@ -5734,7 +5733,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="46" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A46" s="16" t="s">
         <v>14</v>
       </c>
@@ -5769,7 +5768,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="47" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A47" s="16" t="s">
         <v>28</v>
       </c>
@@ -5807,7 +5806,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:13" s="16" customFormat="1" ht="15.75">
+    <row r="48" spans="1:13" s="16" customFormat="1" ht="16">
       <c r="A48" s="16" t="s">
         <v>14</v>
       </c>
@@ -5842,7 +5841,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:25" s="16" customFormat="1" ht="15.75">
+    <row r="49" spans="1:25" s="16" customFormat="1" ht="16">
       <c r="A49" s="16" t="s">
         <v>14</v>
       </c>
@@ -5877,7 +5876,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:25" s="16" customFormat="1" ht="15.75">
+    <row r="50" spans="1:25" s="16" customFormat="1" ht="16">
       <c r="A50" s="16" t="s">
         <v>14</v>
       </c>
@@ -5912,7 +5911,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:25" s="16" customFormat="1" ht="15.75">
+    <row r="51" spans="1:25" s="16" customFormat="1" ht="16">
       <c r="A51" s="16" t="s">
         <v>14</v>
       </c>
@@ -5944,7 +5943,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:25" s="16" customFormat="1" ht="15.75">
+    <row r="52" spans="1:25" s="16" customFormat="1" ht="16">
       <c r="A52" s="16" t="s">
         <v>41</v>
       </c>
@@ -5979,7 +5978,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:25" s="16" customFormat="1" ht="15.75">
+    <row r="53" spans="1:25" s="16" customFormat="1" ht="16">
       <c r="A53" s="16" t="s">
         <v>41</v>
       </c>
@@ -6014,7 +6013,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:25" s="16" customFormat="1" ht="15.75">
+    <row r="54" spans="1:25" s="16" customFormat="1" ht="16">
       <c r="A54" s="16" t="s">
         <v>41</v>
       </c>
@@ -6049,7 +6048,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:25" s="16" customFormat="1" ht="15.75">
+    <row r="55" spans="1:25" s="16" customFormat="1" ht="16">
       <c r="A55" s="16" t="s">
         <v>41</v>
       </c>
@@ -6084,7 +6083,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:25" s="16" customFormat="1" ht="15.75">
+    <row r="56" spans="1:25" s="16" customFormat="1" ht="16">
       <c r="A56" s="16" t="s">
         <v>41</v>
       </c>
@@ -6119,7 +6118,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:25" s="16" customFormat="1" ht="15.75">
+    <row r="57" spans="1:25" s="16" customFormat="1" ht="16">
       <c r="A57" s="16" t="s">
         <v>41</v>
       </c>
@@ -6154,7 +6153,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:25" s="16" customFormat="1" ht="15.75">
+    <row r="58" spans="1:25" s="16" customFormat="1" ht="16">
       <c r="A58" s="16" t="s">
         <v>41</v>
       </c>
@@ -6189,7 +6188,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:25" s="16" customFormat="1" ht="15.75">
+    <row r="59" spans="1:25" s="16" customFormat="1" ht="16">
       <c r="A59" s="16" t="s">
         <v>41</v>
       </c>
@@ -6224,7 +6223,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="60" spans="1:25" s="16" customFormat="1" ht="15.75">
+    <row r="60" spans="1:25" s="16" customFormat="1" ht="16">
       <c r="A60" s="16" t="s">
         <v>41</v>
       </c>
@@ -6259,7 +6258,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:25" s="16" customFormat="1" ht="15.75">
+    <row r="61" spans="1:25" s="16" customFormat="1" ht="16">
       <c r="A61" s="16" t="s">
         <v>25</v>
       </c>
@@ -6294,7 +6293,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:25" s="16" customFormat="1" ht="15.75">
+    <row r="62" spans="1:25" s="16" customFormat="1" ht="16">
       <c r="A62" s="16" t="s">
         <v>41</v>
       </c>
@@ -6326,7 +6325,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:25" s="16" customFormat="1" ht="15.75">
+    <row r="63" spans="1:25" s="16" customFormat="1" ht="16">
       <c r="A63" s="37" t="s">
         <v>41</v>
       </c>
@@ -6373,7 +6372,7 @@
       <c r="X63" s="37"/>
       <c r="Y63" s="37"/>
     </row>
-    <row r="64" spans="1:25" ht="15.75">
+    <row r="64" spans="1:25" ht="16">
       <c r="A64" s="16" t="s">
         <v>28</v>
       </c>
@@ -6424,7 +6423,7 @@
       <c r="X64" s="11"/>
       <c r="Y64" s="11"/>
     </row>
-    <row r="65" spans="1:23" ht="15.75">
+    <row r="65" spans="1:23" ht="16">
       <c r="A65" s="46" t="s">
         <v>41</v>
       </c>
@@ -6469,7 +6468,7 @@
       <c r="V65" s="40"/>
       <c r="W65" s="40"/>
     </row>
-    <row r="66" spans="1:23" ht="15.75">
+    <row r="66" spans="1:23" ht="16">
       <c r="A66" s="36" t="s">
         <v>41</v>
       </c>
@@ -6514,7 +6513,7 @@
       <c r="V66" s="11"/>
       <c r="W66" s="11"/>
     </row>
-    <row r="67" spans="1:23" ht="15.75">
+    <row r="67" spans="1:23" ht="16">
       <c r="A67" s="36" t="s">
         <v>41</v>
       </c>
@@ -6559,7 +6558,7 @@
       <c r="V67" s="11"/>
       <c r="W67" s="11"/>
     </row>
-    <row r="68" spans="1:23" ht="15.75">
+    <row r="68" spans="1:23" ht="16">
       <c r="A68" s="36" t="s">
         <v>41</v>
       </c>
@@ -6604,7 +6603,7 @@
       <c r="V68" s="11"/>
       <c r="W68" s="11"/>
     </row>
-    <row r="69" spans="1:23" ht="15.75">
+    <row r="69" spans="1:23" ht="16">
       <c r="A69" s="36" t="s">
         <v>41</v>
       </c>
@@ -6661,54 +6660,54 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2:B55"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="76.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="76.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="28" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="61.140625" customWidth="1"/>
-    <col min="16" max="16" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.140625" customWidth="1"/>
+    <col min="14" max="14" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="61.1640625" customWidth="1"/>
+    <col min="16" max="16" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="22" customFormat="1" ht="18.75">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:32" s="22" customFormat="1" ht="19">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="31" t="s">
@@ -9313,7 +9312,7 @@
       <c r="AE47" s="5"/>
       <c r="AF47" s="5"/>
     </row>
-    <row r="48" spans="1:32" ht="15.75">
+    <row r="48" spans="1:32" ht="16">
       <c r="A48" s="6" t="s">
         <v>41</v>
       </c>
@@ -10267,54 +10266,56 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:R75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="64.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.5" style="1" customWidth="1"/>
     <col min="12" max="12" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="28" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.5" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="66" style="1" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="9.140625" style="1"/>
+    <col min="16" max="16" width="16.33203125" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18.75">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:18" ht="19">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="29" t="s">
@@ -12325,7 +12326,7 @@
       </c>
       <c r="P51" s="6"/>
     </row>
-    <row r="52" spans="1:16" ht="15.75" hidden="1">
+    <row r="52" spans="1:16" ht="16" hidden="1">
       <c r="A52" s="57" t="s">
         <v>25</v>
       </c>
@@ -12566,6 +12567,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F02A65CCC60F874B9ADA1BEFF5AA36D9" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eb3e10658d6e9522cdb69c519ad4b761">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="fc2aed38-3608-4b3b-b1cf-95addf4ae31b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="37b0b56e23b33396ae5e88d68df91971" ns2:_="">
     <xsd:import namespace="fc2aed38-3608-4b3b-b1cf-95addf4ae31b"/>
@@ -12709,29 +12725,37 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25C9861B-F4E6-4D20-AE30-B8C44E7E7247}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F759271B-1F90-4B9A-B820-64A6233DF3CC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{551526DD-87C7-4853-9A23-07E0E4973FD1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{551526DD-87C7-4853-9A23-07E0E4973FD1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F759271B-1F90-4B9A-B820-64A6233DF3CC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25C9861B-F4E6-4D20-AE30-B8C44E7E7247}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="fc2aed38-3608-4b3b-b1cf-95addf4ae31b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>